<commit_message>
Solve problem 27 & 28
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="122">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -483,6 +483,24 @@
   </si>
   <si>
     <t xml:space="preserve">9.50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">移除元素</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove-element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">191118-1.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">实现 strStr()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement-strstr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.58%</t>
   </si>
   <si>
     <t xml:space="preserve">最长连续序列</t>
@@ -714,7 +732,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1520,10 +1538,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>113</v>
@@ -1532,18 +1550,76 @@
         <v>114</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" s="4" t="n">
+        <v>36942276</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <v>36942358</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="n">
+        <v>128</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="6" t="n">
+      <c r="F30" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="G28" s="6" t="n">
+      <c r="G30" s="6" t="n">
         <v>10.3</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="4" t="n">
+      <c r="H30" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I30" s="4" t="n">
         <v>31769076</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update solution of 57
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -803,7 +803,7 @@
     <t xml:space="preserve">insert-interval</t>
   </si>
   <si>
-    <t xml:space="preserve">5.88%</t>
+    <t xml:space="preserve">8.33%</t>
   </si>
   <si>
     <t xml:space="preserve">最长连续序列</t>
@@ -2726,16 +2726,16 @@
         <v>210</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>1208</v>
+        <v>316</v>
       </c>
       <c r="G58" s="6" t="n">
-        <v>12.3</v>
+        <v>12.4</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>219</v>
       </c>
       <c r="I58" s="4" t="n">
-        <v>41881074</v>
+        <v>41882354</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Improve solution of 57
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="224">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -803,7 +803,10 @@
     <t xml:space="preserve">insert-interval</t>
   </si>
   <si>
-    <t xml:space="preserve">8.33%</t>
+    <t xml:space="preserve">200101-1.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.85%</t>
   </si>
   <si>
     <t xml:space="preserve">最长连续序列</t>
@@ -1040,7 +1043,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I59" activeCellId="0" sqref="I59"/>
+      <selection pane="bottomLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2723,19 +2726,19 @@
         <v>218</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>316</v>
+        <v>8</v>
       </c>
       <c r="G58" s="6" t="n">
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I58" s="4" t="n">
-        <v>41882354</v>
+        <v>41914872</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,10 +2749,10 @@
         <v>23</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>17</v>
@@ -2761,7 +2764,7 @@
         <v>10.3</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I59" s="4" t="n">
         <v>31769076</v>

</xml_diff>

<commit_message>
Update results of 61
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="237">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -843,6 +843,9 @@
   </si>
   <si>
     <t xml:space="preserve">rotate-list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.86%</t>
   </si>
   <si>
     <t xml:space="preserve">最长连续序列</t>
@@ -1077,9 +1080,9 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F62" activeCellId="0" sqref="F62"/>
+      <selection pane="bottomLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2880,10 +2883,18 @@
       <c r="E62" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="4"/>
+      <c r="F62" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G62" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="I62" s="4" t="n">
+        <v>42398520</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="n">
@@ -2893,10 +2904,10 @@
         <v>23</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>17</v>
@@ -2908,7 +2919,7 @@
         <v>10.3</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I63" s="4" t="n">
         <v>31769076</v>

</xml_diff>

<commit_message>
Solve 66 & 67
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="254">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -885,6 +885,18 @@
   </si>
   <si>
     <t xml:space="preserve">87.72%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">加一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plus-one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">二进制求和</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add-binary</t>
   </si>
   <si>
     <t xml:space="preserve">最长连续序列</t>
@@ -1116,12 +1128,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I67" activeCellId="0" sqref="I67"/>
+      <selection pane="bottomLeft" activeCell="I69" activeCellId="0" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3053,10 +3065,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="n">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>247</v>
@@ -3065,18 +3077,76 @@
         <v>248</v>
       </c>
       <c r="E67" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F67" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" s="6" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I67" s="4" t="n">
+        <v>42668177</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F68" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="6" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I68" s="4" t="n">
+        <v>42668665</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="4" t="n">
+        <v>128</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F67" s="6" t="n">
+      <c r="F69" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="G67" s="6" t="n">
+      <c r="G69" s="6" t="n">
         <v>10.3</v>
       </c>
-      <c r="H67" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="I67" s="4" t="n">
+      <c r="H69" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="I69" s="4" t="n">
         <v>31769076</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solve 175 & 176
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="584">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -1875,6 +1875,27 @@
   </si>
   <si>
     <t xml:space="preserve">79.51%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">组合两个表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combine-two-tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200221-1.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.84%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">第二高的薪水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second-highest-salary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.64%</t>
   </si>
 </sst>
 </file>
@@ -2105,12 +2126,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I169" activeCellId="0" sqref="I169"/>
+      <selection pane="bottomLeft" activeCell="I171" activeCellId="0" sqref="I171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6997,6 +7018,64 @@
         <v>48466281</v>
       </c>
     </row>
+    <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A169" s="6" t="n">
+        <v>175</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="D169" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="F169" s="8" t="n">
+        <v>176</v>
+      </c>
+      <c r="G169" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="I169" s="6" t="n">
+        <v>48466380</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A170" s="6" t="n">
+        <v>176</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="D170" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="F170" s="8" t="n">
+        <v>181</v>
+      </c>
+      <c r="G170" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="I170" s="6" t="n">
+        <v>48466681</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Update 175 & 176
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="585">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -1886,7 +1886,7 @@
     <t xml:space="preserve">200221-1.sql</t>
   </si>
   <si>
-    <t xml:space="preserve">41.84%</t>
+    <t xml:space="preserve">86.70%</t>
   </si>
   <si>
     <t xml:space="preserve">第二高的薪水</t>
@@ -1895,7 +1895,10 @@
     <t xml:space="preserve">second-highest-salary</t>
   </si>
   <si>
-    <t xml:space="preserve">10.64%</t>
+    <t xml:space="preserve">200224-1.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.54%</t>
   </si>
 </sst>
 </file>
@@ -2140,9 +2143,9 @@
   <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I171" activeCellId="0" sqref="I171"/>
+      <selection pane="bottomLeft" activeCell="A171" activeCellId="0" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7046,7 +7049,7 @@
         <v>579</v>
       </c>
       <c r="F169" s="8" t="n">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G169" s="8" t="n">
         <v>0</v>
@@ -7055,7 +7058,7 @@
         <v>580</v>
       </c>
       <c r="I169" s="6" t="n">
-        <v>48466380</v>
+        <v>49076028</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7072,19 +7075,19 @@
         <v>582</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="F170" s="8" t="n">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="G170" s="8" t="n">
         <v>0</v>
       </c>
       <c r="H170" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="I170" s="6" t="n">
-        <v>48466681</v>
+        <v>49076446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to solve 282
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="848">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -2676,6 +2676,18 @@
   </si>
   <si>
     <t xml:space="preserve">67.13%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">给表达式添加运算符</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expression-add-operators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200706-2.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
 </sst>
 </file>
@@ -2918,15 +2930,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J247"/>
+  <dimension ref="A1:J248"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E248" activeCellId="0" sqref="E248"/>
+      <selection pane="bottomLeft" activeCell="E249" activeCellId="0" sqref="E249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.25"/>
@@ -10361,6 +10373,36 @@
       </c>
       <c r="J247" s="13"/>
     </row>
+    <row r="248" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="7" t="n">
+        <v>282</v>
+      </c>
+      <c r="B248" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>844</v>
+      </c>
+      <c r="D248" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="E248" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="F248" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="G248" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="H248" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="I248" s="8" t="s">
+        <v>847</v>
+      </c>
+      <c r="J248" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Try to solve 354
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1004">
   <si>
     <t xml:space="preserve">编号</t>
   </si>
@@ -3147,6 +3147,15 @@
   </si>
   <si>
     <t xml:space="preserve">88.94%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">俄罗斯套娃信封问题</t>
+  </si>
+  <si>
+    <t xml:space="preserve">russian-doll-envelopes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201025-1.cpp</t>
   </si>
 </sst>
 </file>
@@ -3393,15 +3402,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K287"/>
+  <dimension ref="A1:K288"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J288" activeCellId="0" sqref="J288"/>
+      <selection pane="bottomLeft" activeCell="E289" activeCellId="0" sqref="E289"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.25"/>
@@ -12869,6 +12878,29 @@
       </c>
       <c r="K287" s="13"/>
     </row>
+    <row r="288" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A288" s="7" t="n">
+        <v>354</v>
+      </c>
+      <c r="B288" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C288" s="9" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D288" s="10" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E288" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F288" s="9"/>
+      <c r="G288" s="9"/>
+      <c r="H288" s="11"/>
+      <c r="I288" s="11"/>
+      <c r="J288" s="7"/>
+      <c r="K288" s="13"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>